<commit_message>
Feat : Load 함수 구현
- 드롭 프리펩 오류
</commit_message>
<xml_diff>
--- a/Survival/Assets/Excel/MonsterSheet.xlsx
+++ b/Survival/Assets/Excel/MonsterSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\조윤진\Documents\GitHub\Survival\Survival\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819D663E-684B-40CB-ADA9-CAFE859869AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841CCE62-5667-4A8C-85ED-47943713CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14303" yWindow="-5558" windowWidth="21795" windowHeight="12975" xr2:uid="{89C4C4D7-03BA-4731-AEC5-6C121413ADA1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89C4C4D7-03BA-4731-AEC5-6C121413ADA1}"/>
   </bookViews>
   <sheets>
     <sheet name="MonsterData" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
   <si>
     <t>Health</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,19 +90,34 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> Monster/1/Blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monster/1/Red</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monster/1/Red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> Monster/1/Green</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Monster/1/Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster/1/Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster/1/Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Monster/2/Red</t>
+  </si>
+  <si>
+    <t>Monster/3/Red</t>
+  </si>
+  <si>
+    <t>Monster/4/Red</t>
+  </si>
+  <si>
+    <t>Monster/5/Red</t>
+  </si>
+  <si>
+    <t>Monster/6/Red</t>
+  </si>
+  <si>
+    <t>Monster/7/Red</t>
   </si>
 </sst>
 </file>
@@ -501,7 +516,7 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -587,7 +602,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -639,7 +654,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -665,7 +680,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -691,7 +706,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -717,7 +732,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -743,7 +758,7 @@
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -769,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix : 몬스터 Load 함수
</commit_message>
<xml_diff>
--- a/Survival/Assets/Excel/MonsterSheet.xlsx
+++ b/Survival/Assets/Excel/MonsterSheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\조윤진\Documents\GitHub\Survival\Survival\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841CCE62-5667-4A8C-85ED-47943713CDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2247955C-48C9-4141-8A60-28102C52F680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89C4C4D7-03BA-4731-AEC5-6C121413ADA1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Health</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,34 +90,56 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Monster/1/Blue</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster/1/Green</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster/1/Red</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Monster/2/Red</t>
-  </si>
-  <si>
-    <t>Monster/3/Red</t>
-  </si>
-  <si>
-    <t>Monster/4/Red</t>
-  </si>
-  <si>
-    <t>Monster/5/Red</t>
-  </si>
-  <si>
-    <t>Monster/6/Red</t>
-  </si>
-  <si>
-    <t>Monster/7/Red</t>
+    <t>StegaGreen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StegaPurple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RaptoGreen</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RaptoOrange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/1/Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/1/Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/1/Red</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/2/Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/2/Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/2/Purple</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/3/Blue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/3/Green</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Monster/3/Orange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -515,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8E3C918-7E62-4F53-8273-05DF0D4D41A4}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -576,7 +598,7 @@
         <v>10</v>
       </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -602,7 +624,7 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -628,7 +650,7 @@
         <v>10</v>
       </c>
       <c r="H4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -654,7 +676,7 @@
         <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -665,7 +687,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D6" s="1">
         <v>100</v>
@@ -680,7 +702,7 @@
         <v>10</v>
       </c>
       <c r="H6" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -691,7 +713,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7" s="1">
         <v>100</v>
@@ -706,7 +728,7 @@
         <v>10</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -732,7 +754,7 @@
         <v>10</v>
       </c>
       <c r="H8" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -743,7 +765,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>200</v>
@@ -758,7 +780,7 @@
         <v>10</v>
       </c>
       <c r="H9" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -769,7 +791,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D10" s="1">
         <v>200</v>
@@ -784,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="H10" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>